<commit_message>
Update COURSES CHEVAUX Matrice.xlsx
</commit_message>
<xml_diff>
--- a/103_BaseDeDonnees/Exercices/203_CourseChevaux/COURSES CHEVAUX Matrice.xlsx
+++ b/103_BaseDeDonnees/Exercices/203_CourseChevaux/COURSES CHEVAUX Matrice.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcravo\Documents\GitHub\FORMATION-CDA-2210\103_BaseDeDonnees\Exercices\203_CourseChevaux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ba75d8fe6eadcc5e/Documents/GitHub/FORMATION-CDA-2210/103_BaseDeDonnees/Exercices/203_CourseChevaux/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3E77BE-9A8C-4BD4-A8AD-0B8E5AD7D54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{6B3E77BE-9A8C-4BD4-A8AD-0B8E5AD7D54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A14CB04-46A4-4B36-B51F-F693E74BF3B3}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>course_nom</t>
   </si>
@@ -39,25 +39,22 @@
     <t>cheval_numero</t>
   </si>
   <si>
-    <t>cheval_position_arrivee</t>
-  </si>
-  <si>
     <t>pari_id</t>
   </si>
   <si>
     <t>pari_somme</t>
   </si>
   <si>
-    <t>pari_gain</t>
-  </si>
-  <si>
-    <t>pari_cheval_position</t>
-  </si>
-  <si>
-    <t>type_id</t>
-  </si>
-  <si>
-    <t>type_libelle</t>
+    <t>course_resultat</t>
+  </si>
+  <si>
+    <t>pari_ordre</t>
+  </si>
+  <si>
+    <t>categorie_id</t>
+  </si>
+  <si>
+    <t>categorie_libelle</t>
   </si>
 </sst>
 </file>
@@ -144,6 +141,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +422,7 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -432,10 +433,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -461,28 +462,28 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
+      <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5">
@@ -493,7 +494,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -502,7 +503,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -523,15 +524,15 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -539,19 +540,8 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>